<commit_message>
update a lot of function
</commit_message>
<xml_diff>
--- a/public/files/xlsx/example-list-checkin.xlsx
+++ b/public/files/xlsx/example-list-checkin.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\diemdanh-app\public\files\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3150" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="4050" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="DIEMDANH" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -45,13 +45,31 @@
   </si>
   <si>
     <t>toladev.info</t>
+  </si>
+  <si>
+    <t>Gmail</t>
+  </si>
+  <si>
+    <t>c@gmail.com</t>
+  </si>
+  <si>
+    <t>toladev@gmail.com</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>18520847@gm.uit.edu.vn</t>
+  </si>
+  <si>
+    <t>nqh.webdev@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,6 +80,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,10 +137,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -122,8 +149,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,69 +433,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>11111</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>11112</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>11113</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>11114</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>